<commit_message>
ambios reporte excel correcciones
</commit_message>
<xml_diff>
--- a/src/assets/reportes/newExcel1.xlsx
+++ b/src/assets/reportes/newExcel1.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="22">
   <si>
     <t>ID</t>
   </si>
@@ -40,7 +40,7 @@
     <t>UBICACIÓN</t>
   </si>
   <si>
-    <t>pepo</t>
+    <t>pelusa</t>
   </si>
   <si>
     <t>perro</t>
@@ -55,28 +55,28 @@
     <t>Publicado</t>
   </si>
   <si>
+    <t>/assets/recibidas/1.jpg</t>
+  </si>
+  <si>
+    <t>{"lat":-34.60975,"lng":-58.428904}</t>
+  </si>
+  <si>
+    <t>Truman</t>
+  </si>
+  <si>
+    <t>rubio</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>pompon</t>
-  </si>
-  <si>
-    <t>gato</t>
-  </si>
-  <si>
-    <t>gris</t>
-  </si>
-  <si>
-    <t>{"lat":-34.60669,"lng":-58.429266}</t>
-  </si>
-  <si>
-    <t>Truman</t>
-  </si>
-  <si>
-    <t>rubio</t>
-  </si>
-  <si>
-    <t>{}</t>
+    <t>{"lat":-34.613464,"lng":-58.428317}</t>
+  </si>
+  <si>
+    <t>/assets/recibidas/3.jpg</t>
+  </si>
+  <si>
+    <t>/assets/recibidas/4.jpg</t>
   </si>
 </sst>
 </file>
@@ -453,7 +453,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I9"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -485,15 +485,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -509,6 +509,9 @@
       </c>
       <c r="H2" t="s">
         <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -516,13 +519,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
         <v>17</v>
@@ -534,18 +537,18 @@
         <v>13</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="I3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C4">
         <v>4</v>
@@ -554,7 +557,7 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F4" t="s">
         <v>12</v>
@@ -563,10 +566,155 @@
         <v>13</v>
       </c>
       <c r="H4" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="I4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" t="s">
         <v>21</v>
+      </c>
+      <c r="I9" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>